<commit_message>
Fixed duplicate excel bug
</commit_message>
<xml_diff>
--- a/My Form.xlsx
+++ b/My Form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -37,19 +37,19 @@
     <t>Symptoms</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi </t>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Jfjvk</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Meghan</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
@@ -426,27 +426,21 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
@@ -456,7 +450,7 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>